<commit_message>
penambahan agent baru menggunakan RAG data Kambingku betadan external store menggunakan creds.json untuk spreadsheets
</commit_message>
<xml_diff>
--- a/hasil_pencarian_kambing.xlsx
+++ b/hasil_pencarian_kambing.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,6 +576,217 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-08-03 20:32:24</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>list sekolah yang ikut di aplikasi saat ini</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Saya mohon maaf, saat ini saya tidak dapat memberikan daftar sekolah yang berpartisipasi dalam aplikasi "kambingku" karena keterbatasan akses terhadap dataset yang relevan. Data yang diperlukan tidak dapat ditemukan dalam pencarian sebelumnya, dan tampaknya ada masalah dengan akses ke sumber data yang tepat atau kueri pencarian. Untuk informasi lebih lanjut atau pembaruan terkini, saya sarankan untuk mengunjungi situs web resmi aplikasi "kambingku" atau menghubungi pengembang aplikasi tersebut. Jika ada sumber daya atau informasi tambahan yang dapat diakses, saya akan dengan senang hati membantu lebih lanjut.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-08-03 21:28:33</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>berapa jumalh sekolah yang terdaftar</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Berikut adalah jumlah sekolah yang terdaftar dalam aplikasi "kambingku" berdasarkan data yang tersedia:
+1. **Pertanian Kelubir Terpadu (PTK) PT Khatulistiwa Nusantara**
+   - Lokasi: Kelubir, Kec. Tj. Palas Utara, Kabupaten Bulungan, Kalimantan Utara
+   - Kontak: 085348781265
+   - Website: [PTK Goat](https://ptk-goat.gaenitraining.org)
+2. **SMKN 2 INDRAMAYU**
+   - Lokasi: Jl. Raya Pabean Udik No.15, Pabeanudik, Kec. Indramayu, Kabupaten Indramayu, Jawa Barat 45219
+   - Kontak: 0895380266682
+   - Website: [SMKN 2 Indramayu](https://smkn2indramayu.sch.id/)
+3. **FARM RUMAH BELAJAR PRANASISWA**
+   - Website: [Gaeni](https://www.gaeni.org)
+Total jumlah sekolah yang terdaftar adalah **tiga sekolah**. Informasi ini diambil dari file school.csv yang berisi data sekolah-sekolah yang terdaftar dalam aplikasi tersebut.
+Referensi:
+- [PTK Goat](https://ptk-goat.gaenitraining.org)
+- [SMKN 2 Indramayu](https://smkn2indramayu.sch.id/)
+- [Gaeni](https://www.gaeni.org)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-08-03 21:30:17</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>apa aja jenis kambing yang terdata</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>### Jenis-Jenis Kambing
+Kambing adalah hewan ternak yang memiliki berbagai jenis yang tersebar di seluruh dunia. Berikut adalah beberapa jenis kambing yang umum dikenal:
+1. **Kambing Boer**: Kambing ini berasal dari Afrika Selatan dan dikenal karena pertumbuhan yang cepat dan produksi daging yang tinggi. Kambing Boer memiliki tubuh yang besar dan otot yang kuat.
+2. **Kambing Saanen**: Berasal dari Swiss, kambing ini terkenal sebagai penghasil susu yang baik. Kambing Saanen memiliki bulu putih dan ukuran tubuh yang besar.
+3. **Kambing Etawa (Jamnapari)**: Kambing ini berasal dari India dan dikenal karena kemampuan produksi susu yang tinggi. Kambing Etawa juga sering digunakan dalam persilangan untuk meningkatkan kualitas kambing lokal.
+4. **Kambing Kacang**: Jenis kambing lokal Indonesia yang memiliki ukuran tubuh kecil dan tahan terhadap kondisi lingkungan yang keras. Kambing ini sering dipelihara untuk diambil dagingnya.
+5. **Kambing Anglo-Nubian**: Kambing ini adalah hasil persilangan antara kambing Inggris dan kambing dari Timur Tengah. Mereka dikenal karena produksi susu yang tinggi dan kualitas daging yang baik.
+6. **Kambing Alpine**: Berasal dari Pegunungan Alpen, kambing ini dikenal karena produksi susu yang baik dan kemampuan beradaptasi dengan berbagai kondisi iklim.
+7. **Kambing Toggenburg**: Kambing ini berasal dari Swiss dan merupakan salah satu ras kambing perah tertua. Mereka memiliki bulu coklat dengan tanda putih di wajah dan kaki.
+Untuk informasi lebih lanjut mengenai jenis-jenis kambing, Anda dapat mengunjungi [Wikipedia - Goat](https://en.wikipedia.org/wiki/Goat) atau sumber lain yang terpercaya.
+Referensi:
+- [Wikipedia - Goat](https://en.wikipedia.org/wiki/Goat)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-08-03 21:31:51</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>berikan aku data kambing dengan jenis etawa</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>### Kambing Etawa
+Kambing Etawa, juga dikenal sebagai kambing Jamnapari, adalah salah satu jenis kambing yang berasal dari India dan telah banyak dibudidayakan di Indonesia. Kambing ini terkenal karena ukuran tubuhnya yang besar dan kemampuan produksinya yang baik, baik untuk susu maupun daging.
+#### Ciri-ciri Kambing Etawa:
+- **Ukuran Tubuh:** Kambing Etawa memiliki tubuh yang besar dengan tinggi mencapai 90-100 cm untuk jantan dan 70-90 cm untuk betina.
+- **Berat Badan:** Berat kambing jantan dewasa bisa mencapai 91 kg, sedangkan betina sekitar 63 kg.
+- **Bulu:** Memiliki bulu yang panjang dan lebat, terutama di bagian paha dan punggung. Warna bulu bervariasi, tetapi umumnya berwarna putih dengan bercak coklat atau hitam.
+- **Telinga:** Telinga panjang dan menggantung, menjadi salah satu ciri khas kambing ini.
+- **Produksi Susu:** Kambing Etawa dikenal sebagai penghasil susu yang baik, dengan produksi susu harian bisa mencapai 3-4 liter.
+- **Adaptasi:** Kambing ini mampu beradaptasi dengan baik di berbagai kondisi iklim, membuatnya populer di berbagai daerah di Indonesia.
+#### Manfaat:
+- **Susu:** Susu kambing Etawa kaya akan nutrisi dan sering digunakan sebagai alternatif susu sapi, terutama bagi mereka yang alergi terhadap laktosa.
+- **Daging:** Selain susu, kambing ini juga dipelihara untuk dagingnya yang berkualitas tinggi.
+- **Pembiakan:** Kambing Etawa sering digunakan dalam program pembiakan untuk meningkatkan kualitas genetik kambing lokal.
+#### Pemeliharaan:
+- **Pakan:** Kambing Etawa memerlukan pakan berkualitas tinggi yang kaya akan protein dan serat untuk mendukung pertumbuhannya.
+- **Kandang:** Kandang harus bersih dan cukup luas untuk mendukung aktivitas kambing, serta dilengkapi dengan sistem drainase yang baik untuk menjaga kebersihan.
+- **Kesehatan:** Perlu dilakukan pemeriksaan kesehatan secara rutin untuk mencegah penyakit dan memastikan produktivitas kambing tetap optimal.
+Untuk informasi lebih lanjut tentang kambing Etawa, Anda bisa mengunjungi [sumber referensi](https://id.wikipedia.org/wiki/Kambing_Etawa).
+Referensi:
+- [Wikipedia: Kambing Etawa](https://id.wikipedia.org/wiki/Kambing_Etawa)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-08-05 08:58:57</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Apa itu Kambing</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>### Apa Itu Kambing?
+Kambing adalah hewan ternak yang termasuk dalam keluarga Bovidae dan subfamili Caprinae. Nama ilmiah kambing adalah *Capra aegagrus hircus*. Kambing telah didomestikasi sejak ribuan tahun yang lalu dan memiliki peran penting dalam kehidupan manusia, baik sebagai sumber daging, susu, kulit, maupun bulu. 
+Kambing dikenal sebagai hewan yang adaptif dan dapat hidup di berbagai lingkungan, dari padang rumput hingga daerah berbatu. Mereka memiliki kemampuan merumput yang baik dan sering digunakan untuk membantu mengendalikan pertumbuhan vegetasi yang berlebihan.
+Di Indonesia, terdapat berbagai jenis kambing yang dibudidayakan, antara lain kambing kacang, kambing etawa, dan kambing peranakan etawa. Setiap jenis memiliki karakteristik dan keunggulan tersendiri, seperti produksi susu yang tinggi atau kemampuan adaptasi yang baik terhadap lingkungan lokal.
+Untuk informasi lebih lanjut mengenai kambing, Anda dapat mengunjungi sumber-sumber berikut:
+- [Kambing - Wikipedia bahasa Indonesia, ensiklopedia bebas](https://id.wikipedia.org/wiki/Kambing)
+- [Nama Ilmiah Kambing dan Jenis-Jenis Kambing yang Ada di Indonesia - Kompas.com](https://www.kompas.com/sains/read/2022/01/07/174600923/nama-ilmiah-kambing-dan-jenis-jenis-kambing-yang-ada-di-indonesia)
+- [PEMUDA PETERNAK KAMBING BUNGKARAN - Pagersari](http://pagersari-patean.desa.id/potensidetail/eUVvYlZFYmdhZDU2dDhJMEFrSm40dz09/pemuda-peternak-kambing-bungkaran.html)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-08-05 08:59:28</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Apa yang cocok sebagai tambahan pakan untuk kambing</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>### Pakan Tambahan yang Cocok untuk Kambing
+Kambing membutuhkan pakan yang seimbang untuk mendukung pertumbuhan dan kesehatannya. Selain pakan utama berupa rumput dan hijauan, ada beberapa jenis pakan tambahan yang dapat diberikan kepada kambing untuk memenuhi kebutuhan nutrisinya:
+1. **Konsentrat**: Konsentrat merupakan pakan tambahan yang penting untuk kambing, terutama untuk meningkatkan produksi susu dan daging. Konsentrat sebaiknya diberikan dalam bentuk kasar agar mudah dicerna oleh kambing. [Baca selengkapnya di sini](https://bbppkupang.bppsdmp.pertanian.go.id/blog/trik-memberikan-pakan-kambing-potong-yang-benar).
+2. **Hijauan dan Dedaunan**: Pakan hijauan seperti rumput gajah, daun singkong, dan kaliandra sangat bagus untuk kambing karena kaya akan serat dan nutrisi. Dedaunan dari tanaman leguminosa seperti turi dan gamal juga dapat menjadi pilihan yang baik. [Baca selengkapnya di sini](https://fpp.umko.ac.id/2021/06/23/jenis-pakan-hijauan-yang-bagus-untuk-kambing/).
+3. **Biji-bijian**: Biji-bijian seperti jagung dan kedelai dapat diberikan sebagai sumber energi tambahan, terutama untuk anakan kambing yang membutuhkan lebih banyak energi untuk pertumbuhan. [Baca selengkapnya di sini](https://www.agropustaka.id/kabar/tips-pemberian-pakan-kambing-dan-domba/).
+4. **Ampas Hasil Pertanian**: Ampas seperti ampas tahu dan ampas bir dapat digunakan sebagai pakan tambahan yang ekonomis dan kaya nutrisi. [Baca selengkapnya di sini](https://gdm.id/pakan-kambing-selain-rumput/).
+5. **Fermentasi Pakan**: Fermentasi pakan dapat meningkatkan kecernaan dan nilai gizi pakan. Ini bisa menjadi pilihan baik saat hijauan sulit didapatkan. [Baca selengkapnya di sini](https://gdm.id/pakan-kambing-selain-rumput/).
+Dengan memberikan pakan tambahan yang tepat, peternak dapat memastikan kambing mendapatkan nutrisi yang cukup untuk pertumbuhan, produksi, dan kesehatannya. Pastikan untuk selalu menyesuaikan jenis dan jumlah pakan dengan kebutuhan spesifik kambing Anda.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-08-05 09:01:42</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>kambing jenis apa yang paling banyak di kambingku?</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Berdasarkan informasi yang tersedia, saya belum dapat menemukan data spesifik mengenai jenis kambing yang paling banyak di aplikasi "Kambingku". Data yang relevan mungkin tersebar di berbagai file seperti `goat.csv` dan `type.csv`. Untuk mendapatkan jawaban yang lebih akurat, disarankan untuk melakukan analisis langsung pada data yang terdapat dalam file-file tersebut, dengan fokus pada kolom yang menunjukkan jenis kambing dan jumlahnya. Analisis ini dapat dilakukan dengan menggunakan perangkat lunak pengolah data seperti Microsoft Excel atau Google Sheets untuk mengidentifikasi jenis kambing yang paling banyak berdasarkan jumlah kemunculannya dalam dataset tersebut.
+Sebagai langkah awal, Anda dapat membuka file `goat.csv` dan `type.csv`, kemudian mencari kolom yang relevan seperti "jenis kambing" dan "jumlah". Setelah itu, lakukan pengelompokan dan penghitungan untuk menemukan jenis kambing yang paling banyak. Jika Anda memerlukan panduan lebih lanjut tentang cara melakukan analisis data ini, Anda dapat mengunjungi sumber daya online atau tutorial yang tersedia.
+Untuk informasi lebih lanjut dan panduan tentang cara melakukan analisis data, Anda dapat mengunjungi [tutorial analisis data dengan Excel](https://support.microsoft.com/id-id/excel) atau [Google Sheets](https://support.google.com/docs/answer/3093480?hl=id).
+Referensi:
+- [Microsoft Excel Support](https://support.microsoft.com/id-id/excel)
+- [Google Sheets Support](https://support.google.com/docs/answer/3093480?hl=id)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-08-05 14:14:57</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Berikan aku rekomendasi pakan selain hijauan untuk kambing</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Berikut adalah beberapa rekomendasi pakan alternatif untuk kambing selain hijauan:
+1. **Dahan dan Batang**: Kambing menyukai makan dahan dan batang, yang dapat ditempatkan di tempat pakan jerami. Ini termasuk buah sumac dan dahan pohon lainnya.
+   - Sumber: [The Renaissance Housewife](https://therenaissancehousewife.weebly.com/home/alternative-goat-feed)
+2. **Jagung**: Sering disebut sebagai "permen kambing," jagung adalah suplemen energi yang sangat baik. Jagung murah dan dapat digunakan untuk mengumpulkan, memindahkan, dan mengandangkan kambing.
+   - Sumber: [Val Verde County](https://valverde.agrilife.org/files/2020/11/Supplementation-of-Grazing-Goats.pdf)
+3. **Ampas Bit atau Kulit Kedelai**: Ini adalah suplemen serat yang dapat difermentasi yang dapat digunakan ketika sumber energi tambahan dibutuhkan, seperti selama kehamilan atau awal laktasi.
+   - Sumber: [Merck Veterinary Manual](https://www.merckvetmanual.com/management-and-nutrition/preventative-health-care-and-husbandry-of-goats/nutrition-of-goats)
+4. **Konsentrat**: Biji-bijian atau konsentrat harus diberikan kepada kambing dengan kebutuhan energi yang lebih tinggi, seperti anak kambing yang sedang tumbuh, kambing hamil, atau menyusui. Penting untuk menyeimbangkan ini dengan kebutuhan nutrisi spesifik kambing.
+   - Sumber: [University of Tennessee](https://vetmed.tennessee.edu/wp-content/uploads/sites/4/UTCVM_LACS-FeedingGoats.pdf)
+5. **Biji Kapas Utuh dan Tepung Kedelai**: Ini adalah pilihan pakan tinggi protein yang dapat digunakan untuk kambing betina menyusui dan kambing lainnya yang membutuhkan asupan protein lebih tinggi.
+   - Sumber: [North Carolina State University](https://content.ces.ncsu.edu/nutritional-feeding-management-of-meat-goats)
+Pilihan-pilihan ini menyediakan berbagai nutrisi dan dapat digunakan untuk melengkapi atau menggantikan pakan hijauan tradisional tergantung pada kebutuhan spesifik kambing.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>